<commit_message>
Update protocol and refactor streaming data
</commit_message>
<xml_diff>
--- a/Document/Protocol.xlsx
+++ b/Document/Protocol.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="194">
   <si>
     <t xml:space="preserve">Abbreviation List</t>
   </si>
@@ -401,7 +401,7 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>0x10</t>
+    <t>0x00</t>
   </si>
   <si>
     <t>DAT_ACC</t>
@@ -434,169 +434,190 @@
     </r>
   </si>
   <si>
+    <t>0x01</t>
+  </si>
+  <si>
+    <t>DAT_ANG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angular velocity</t>
+  </si>
+  <si>
+    <t>rad/s</t>
+  </si>
+  <si>
+    <t>DAT_MAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magnetic field</t>
+  </si>
+  <si>
+    <t>mG</t>
+  </si>
+  <si>
+    <t>DAT_PRES</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>Pa</t>
+  </si>
+  <si>
+    <t>0x04</t>
+  </si>
+  <si>
+    <t>DAT_TEMP</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>0x05</t>
+  </si>
+  <si>
+    <t>DAT_RAW_ACC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw acceleration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw ACC measurement without calibration in sensor frame</t>
+  </si>
+  <si>
+    <t>0x06</t>
+  </si>
+  <si>
+    <t>DAT_RAW_ANG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw angular velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw GYRO measurement without calibration in sensor frame</t>
+  </si>
+  <si>
+    <t>0x07</t>
+  </si>
+  <si>
+    <t>DAT_RAW_MAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw magnetic field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raw MAG measurement without calibration in sensor frame</t>
+  </si>
+  <si>
+    <t>0x10</t>
+  </si>
+  <si>
+    <t>DAT_KF_QUAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KF quaternion</t>
+  </si>
+  <si>
+    <t>float[4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalman-filtered quaternion</t>
+  </si>
+  <si>
     <t>0x11</t>
   </si>
   <si>
-    <t>DAT_GYRO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angular velocity</t>
-  </si>
-  <si>
-    <t>rad/s</t>
+    <t>DAT_KF_RPY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KF RPY</t>
+  </si>
+  <si>
+    <t>rad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalman-filtered RPY</t>
   </si>
   <si>
     <t>0x12</t>
   </si>
   <si>
-    <t>DAT_MAG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Magnetic field</t>
-  </si>
-  <si>
-    <t>mG</t>
+    <t>DAT_KF_VEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KF velocity</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalman-filtered velocity in inertial frame</t>
   </si>
   <si>
     <t>0x13</t>
   </si>
   <si>
-    <t>DAT_PRES</t>
-  </si>
-  <si>
-    <t>Pressure</t>
-  </si>
-  <si>
-    <t>float</t>
-  </si>
-  <si>
-    <t>Pa</t>
+    <t>DAT_KF_POS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KF Position</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalman-filtered position in inertial frame</t>
   </si>
   <si>
     <t>0x14</t>
   </si>
   <si>
-    <t>DAT_TEMP</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>°C</t>
+    <t>DAT_EXT_ACC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External acceleration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External acceleration (acceleration - gravity)</t>
   </si>
   <si>
     <t>0x15</t>
   </si>
   <si>
-    <t>DAT_RAW_ACC_MEAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raw ACC measurement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raw ACC measurement without calibration in sensor frame</t>
+    <t>DAT_ACC_MAG_QUAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quaternion measurment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quaternion calculated from ACC and MAG measurements</t>
   </si>
   <si>
     <t>0x16</t>
   </si>
   <si>
-    <t>DAT_RAW_GYRO_MEAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raw GYRO measurement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raw GYRO measurement without calibration in sensor frame</t>
+    <t>DAT_ACC_MAG_RPY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPY measurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPY calculated from ACC and MAG measurements</t>
   </si>
   <si>
     <t>0x17</t>
   </si>
   <si>
-    <t>DAT_RAW_MAG_MEAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raw MAG measurement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Raw MAG measurement without calibration in sensor frame</t>
-  </si>
-  <si>
-    <t>0x20</t>
-  </si>
-  <si>
-    <t>DAT_KF_RPY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KF RPY</t>
-  </si>
-  <si>
-    <t>rad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPY calculated by KF</t>
-  </si>
-  <si>
-    <t>0x21</t>
-  </si>
-  <si>
-    <t>DAT_KF_ACC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KF acceleration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acceleration in inertial frame calculated from KF RPY and acceleration</t>
-  </si>
-  <si>
-    <t>0x22</t>
-  </si>
-  <si>
-    <t>DAT_KF_VEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KF velocity</t>
-  </si>
-  <si>
-    <t>m/s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Velocity in inertial frame calculated by KF</t>
-  </si>
-  <si>
-    <t>0x23</t>
-  </si>
-  <si>
-    <t>DAT_KF_POS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KF Position</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Position in inertial frame calculated by KF</t>
-  </si>
-  <si>
-    <t>0x24</t>
-  </si>
-  <si>
-    <t>DAT_ACC_RPY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACC RPY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPY calculated from ACC measurement</t>
-  </si>
-  <si>
-    <t>0x25</t>
-  </si>
-  <si>
     <t>DAT_BARO_HEIGHT</t>
   </si>
   <si>
-    <t xml:space="preserve">BARO height</t>
+    <t xml:space="preserve">Height measurement</t>
   </si>
   <si>
     <t xml:space="preserve">Height in inertial frame calculated from BARO measurement</t>
@@ -854,7 +875,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1012,12 +1033,6 @@
     </xf>
     <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2231,7 +2246,6 @@
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
       <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
       <c r="F21" s="37"/>
       <c r="G21" s="37"/>
       <c r="H21" s="22"/>
@@ -2885,10 +2899,10 @@
       <c r="C9" s="31">
         <v>12</v>
       </c>
-      <c r="D9" s="56" t="s">
+      <c r="D9" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="E9" s="56" t="s">
+      <c r="E9" s="31" t="s">
         <v>128</v>
       </c>
       <c r="F9" s="31" t="s">
@@ -2906,10 +2920,10 @@
       <c r="C10" s="31">
         <v>12</v>
       </c>
-      <c r="D10" s="56" t="s">
+      <c r="D10" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="E10" s="56" t="s">
+      <c r="E10" s="31" t="s">
         <v>133</v>
       </c>
       <c r="F10" s="31" t="s">
@@ -2922,79 +2936,79 @@
     </row>
     <row r="11" ht="14.25">
       <c r="B11" s="31" t="s">
-        <v>135</v>
+        <v>25</v>
       </c>
       <c r="C11" s="31">
         <v>12</v>
       </c>
-      <c r="D11" s="56" t="s">
+      <c r="D11" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="31" t="s">
         <v>136</v>
-      </c>
-      <c r="E11" s="56" t="s">
-        <v>137</v>
       </c>
       <c r="F11" s="31" t="s">
         <v>129</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H11" s="34"/>
     </row>
     <row r="12" ht="14.25">
       <c r="B12" s="31" t="s">
-        <v>139</v>
+        <v>42</v>
       </c>
       <c r="C12" s="31">
         <v>4</v>
       </c>
       <c r="D12" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="G12" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="H12" s="34"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="B13" s="31" t="s">
         <v>142</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>143</v>
-      </c>
-      <c r="H12" s="34"/>
-    </row>
-    <row r="13" ht="14.25">
-      <c r="B13" s="56" t="s">
-        <v>144</v>
       </c>
       <c r="C13" s="31">
         <v>4</v>
       </c>
       <c r="D13" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="G13" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="H13" s="34"/>
+    </row>
+    <row r="14" ht="14.25" customHeight="1">
+      <c r="B14" s="31" t="s">
         <v>146</v>
-      </c>
-      <c r="F13" s="56" t="s">
-        <v>142</v>
-      </c>
-      <c r="G13" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="H13" s="34"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="B14" s="56" t="s">
-        <v>148</v>
       </c>
       <c r="C14" s="31">
         <v>12</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>129</v>
@@ -3002,22 +3016,22 @@
       <c r="G14" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="H14" s="57" t="s">
-        <v>151</v>
+      <c r="H14" s="34" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="B15" s="56" t="s">
-        <v>152</v>
+      <c r="B15" s="31" t="s">
+        <v>150</v>
       </c>
       <c r="C15" s="31">
         <v>12</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F15" s="31" t="s">
         <v>129</v>
@@ -3025,207 +3039,248 @@
       <c r="G15" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="H15" s="57" t="s">
-        <v>155</v>
+      <c r="H15" s="34" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="16" ht="14.25">
-      <c r="B16" s="56" t="s">
-        <v>156</v>
+      <c r="B16" s="31" t="s">
+        <v>154</v>
       </c>
       <c r="C16" s="31">
         <v>12</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F16" s="31" t="s">
         <v>129</v>
       </c>
       <c r="G16" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="H16" s="57" t="s">
-        <v>159</v>
+        <v>137</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="17" ht="14.25">
       <c r="B17" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="C17" s="31">
+        <v>16</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="E17" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="C17" s="31">
-        <v>12</v>
-      </c>
-      <c r="D17" s="31" t="s">
+      <c r="F17" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="E17" s="31" t="s">
+      <c r="G17" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="F17" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="G17" s="31" t="s">
+    </row>
+    <row r="18" ht="14.25">
+      <c r="B18" s="31" t="s">
         <v>163</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="18" ht="28.5">
-      <c r="B18" s="31" t="s">
-        <v>165</v>
       </c>
       <c r="C18" s="31">
         <v>12</v>
       </c>
-      <c r="D18" s="51" t="s">
-        <v>166</v>
-      </c>
-      <c r="E18" s="51" t="s">
-        <v>167</v>
+      <c r="D18" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="E18" s="31" t="s">
+        <v>165</v>
       </c>
       <c r="F18" s="31" t="s">
         <v>129</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="H18" s="57" t="s">
-        <v>168</v>
+        <v>166</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="19" ht="14.25">
       <c r="B19" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C19" s="31">
         <v>12</v>
       </c>
       <c r="D19" s="51" t="s">
+        <v>169</v>
+      </c>
+      <c r="E19" s="51" t="s">
         <v>170</v>
-      </c>
-      <c r="E19" s="51" t="s">
-        <v>171</v>
       </c>
       <c r="F19" s="31" t="s">
         <v>129</v>
       </c>
       <c r="G19" s="31" t="s">
+        <v>171</v>
+      </c>
+      <c r="H19" s="34" t="s">
         <v>172</v>
-      </c>
-      <c r="H19" s="34" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="20" ht="14.25">
       <c r="B20" s="31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C20" s="31">
         <v>12</v>
       </c>
       <c r="D20" s="51" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" s="51" t="s">
         <v>175</v>
-      </c>
-      <c r="E20" s="51" t="s">
-        <v>176</v>
       </c>
       <c r="F20" s="31" t="s">
         <v>129</v>
       </c>
       <c r="G20" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="H20" s="34" t="s">
         <v>177</v>
-      </c>
-      <c r="H20" s="34" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="21" ht="14.25">
       <c r="B21" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C21" s="31">
         <v>12</v>
       </c>
       <c r="D21" s="51" t="s">
+        <v>179</v>
+      </c>
+      <c r="E21" s="51" t="s">
         <v>180</v>
-      </c>
-      <c r="E21" s="51" t="s">
-        <v>181</v>
       </c>
       <c r="F21" s="31" t="s">
         <v>129</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>163</v>
+        <v>130</v>
       </c>
       <c r="H21" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" ht="14.25">
       <c r="B22" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22" s="31">
+        <v>16</v>
+      </c>
+      <c r="D22" s="51" t="s">
         <v>183</v>
       </c>
-      <c r="C22" s="31">
+      <c r="E22" s="51" t="s">
+        <v>184</v>
+      </c>
+      <c r="F22" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="G22" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="34" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="B23" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="C23" s="31">
+        <v>12</v>
+      </c>
+      <c r="D23" s="51" t="s">
+        <v>187</v>
+      </c>
+      <c r="E23" s="51" t="s">
+        <v>188</v>
+      </c>
+      <c r="F23" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="G23" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="H23" s="34" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="B24" s="31" t="s">
+        <v>190</v>
+      </c>
+      <c r="C24" s="31">
         <v>4</v>
       </c>
-      <c r="D22" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="E22" s="31" t="s">
-        <v>185</v>
-      </c>
-      <c r="F22" s="31" t="s">
-        <v>142</v>
-      </c>
-      <c r="G22" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="H22" s="34" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="23" ht="14.25">
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="38"/>
-    </row>
-    <row r="24" ht="14.25">
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="38"/>
+      <c r="D24" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="G24" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="H24" s="34" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="25" ht="14.25">
       <c r="B25" s="22"/>
       <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
       <c r="H25" s="38"/>
     </row>
     <row r="26" ht="14.25">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
       <c r="H26" s="38"/>
     </row>
-    <row r="27" ht="14.25"/>
+    <row r="27" ht="14.25">
+      <c r="B27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="H27" s="38"/>
+    </row>
     <row r="28" ht="14.25">
       <c r="H28" s="38"/>
     </row>
-    <row r="35" ht="14.25">
-      <c r="C35" s="38"/>
+    <row r="29" ht="14.25"/>
+    <row r="30" ht="14.25">
+      <c r="H30" s="38"/>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="C37" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add attitude estimation based on measurments
</commit_message>
<xml_diff>
--- a/Document/Protocol.xlsx
+++ b/Document/Protocol.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="1" state="visible" r:id="rId1"/>
@@ -742,7 +742,7 @@
     <t>0x28</t>
   </si>
   <si>
-    <t>DAT_ACC_MAG_QUAT</t>
+    <t>DAT_MEAS_QUAT</t>
   </si>
   <si>
     <t xml:space="preserve">Real part of measured quaternion</t>
@@ -763,7 +763,7 @@
     <t>0x29</t>
   </si>
   <si>
-    <t>DAT_ACC_MAG_RPY</t>
+    <t>DAT_MEAS_RPY</t>
   </si>
   <si>
     <t xml:space="preserve">Measured roll</t>
@@ -1072,7 +1072,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1278,6 +1278,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="18" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3794,7 +3797,7 @@
       <c r="C34" s="33">
         <v>16</v>
       </c>
-      <c r="D34" s="69" t="s">
+      <c r="D34" s="73" t="s">
         <v>233</v>
       </c>
       <c r="E34" s="71" t="s">
@@ -3850,7 +3853,7 @@
       <c r="C38" s="34">
         <v>12</v>
       </c>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="62" t="s">
         <v>240</v>
       </c>
       <c r="E38" s="62" t="s">

</xml_diff>

<commit_message>
Add external acceleration compensation algorithm
</commit_message>
<xml_diff>
--- a/Document/Protocol.xlsx
+++ b/Document/Protocol.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
   <si>
     <t xml:space="preserve">Abbreviation List</t>
   </si>
@@ -607,6 +607,15 @@
   </si>
   <si>
     <t xml:space="preserve">Covariance matrix of measurement noise</t>
+  </si>
+  <si>
+    <t>0x38</t>
+  </si>
+  <si>
+    <t>DAT_HPF_ACC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High-pass filtered acceleration</t>
   </si>
 </sst>
 </file>
@@ -872,7 +881,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="60">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1034,20 +1043,14 @@
     <xf fontId="0" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2997,10 +3000,10 @@
       <c r="D9" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="E9" s="57" t="s">
+      <c r="E9" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="F9" s="58" t="s">
+      <c r="F9" s="31" t="s">
         <v>140</v>
       </c>
       <c r="G9" s="31" t="s">
@@ -3019,10 +3022,10 @@
       <c r="D10" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="F10" s="58" t="s">
+      <c r="F10" s="31" t="s">
         <v>140</v>
       </c>
       <c r="G10" s="31" t="s">
@@ -3041,10 +3044,10 @@
       <c r="D11" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="E11" s="57" t="s">
+      <c r="E11" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="F11" s="58" t="s">
+      <c r="F11" s="31" t="s">
         <v>140</v>
       </c>
       <c r="G11" s="31" t="s">
@@ -3062,10 +3065,10 @@
       <c r="D12" s="31" t="s">
         <v>151</v>
       </c>
-      <c r="E12" s="57" t="s">
+      <c r="E12" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="F12" s="58" t="s">
+      <c r="F12" s="31" t="s">
         <v>140</v>
       </c>
       <c r="G12" s="31" t="s">
@@ -3085,10 +3088,10 @@
       <c r="D13" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="E13" s="57" t="s">
+      <c r="E13" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="F13" s="58" t="s">
+      <c r="F13" s="31" t="s">
         <v>140</v>
       </c>
       <c r="G13" s="31" t="s">
@@ -3108,10 +3111,10 @@
       <c r="D14" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="E14" s="57" t="s">
+      <c r="E14" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="F14" s="58" t="s">
+      <c r="F14" s="31" t="s">
         <v>140</v>
       </c>
       <c r="G14" s="31" t="s">
@@ -3131,10 +3134,10 @@
       <c r="D15" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="E15" s="57" t="s">
+      <c r="E15" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="F15" s="58" t="s">
+      <c r="F15" s="31" t="s">
         <v>165</v>
       </c>
       <c r="G15" s="31" t="s">
@@ -3149,13 +3152,13 @@
       <c r="C16" s="31">
         <v>12</v>
       </c>
-      <c r="D16" s="59" t="s">
+      <c r="D16" s="57" t="s">
         <v>167</v>
       </c>
-      <c r="E16" s="57" t="s">
+      <c r="E16" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="F16" s="58" t="s">
+      <c r="F16" s="31" t="s">
         <v>140</v>
       </c>
       <c r="G16" s="31" t="s">
@@ -3170,13 +3173,13 @@
       <c r="C17" s="31">
         <v>16</v>
       </c>
-      <c r="D17" s="59" t="s">
+      <c r="D17" s="57" t="s">
         <v>171</v>
       </c>
-      <c r="E17" s="60" t="s">
+      <c r="E17" s="52" t="s">
         <v>172</v>
       </c>
-      <c r="F17" s="58" t="s">
+      <c r="F17" s="31" t="s">
         <v>165</v>
       </c>
       <c r="G17" s="31" t="s">
@@ -3193,13 +3196,13 @@
       <c r="C18" s="32">
         <v>12</v>
       </c>
-      <c r="D18" s="57" t="s">
+      <c r="D18" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="E18" s="57" t="s">
+      <c r="E18" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="F18" s="57" t="s">
+      <c r="F18" s="32" t="s">
         <v>140</v>
       </c>
       <c r="G18" s="32" t="s">
@@ -3210,85 +3213,100 @@
       </c>
     </row>
     <row r="19" ht="14.25">
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="32" t="s">
         <v>178</v>
       </c>
       <c r="C19" s="32">
         <v>64</v>
       </c>
-      <c r="D19" s="57" t="s">
+      <c r="D19" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="E19" s="57" t="s">
+      <c r="E19" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="F19" s="57" t="s">
+      <c r="F19" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="G19" s="57" t="s">
+      <c r="G19" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="H19" s="61" t="s">
+      <c r="H19" s="37" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="20" ht="14.25">
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="32" t="s">
         <v>183</v>
       </c>
       <c r="C20" s="32">
         <v>64</v>
       </c>
-      <c r="D20" s="57" t="s">
+      <c r="D20" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="E20" s="57" t="s">
+      <c r="E20" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="F20" s="57" t="s">
+      <c r="F20" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="G20" s="57" t="s">
+      <c r="G20" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="61" t="s">
+      <c r="H20" s="37" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="21" ht="14.25">
-      <c r="B21" s="57" t="s">
+      <c r="B21" s="32" t="s">
         <v>186</v>
       </c>
       <c r="C21" s="32">
         <v>64</v>
       </c>
-      <c r="D21" s="57" t="s">
+      <c r="D21" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="E21" s="57" t="s">
+      <c r="E21" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="F21" s="57" t="s">
+      <c r="F21" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="G21" s="57" t="s">
+      <c r="G21" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="61" t="s">
+      <c r="H21" s="37" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="28" ht="14.25">
-      <c r="C28" s="40"/>
-    </row>
-    <row r="41" ht="14.25">
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="40"/>
+    <row r="22" ht="14.25">
+      <c r="B22" s="58" t="s">
+        <v>189</v>
+      </c>
+      <c r="C22" s="32">
+        <v>12</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>191</v>
+      </c>
+      <c r="F22" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="G22" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="H22" s="37"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="B23" s="59"/>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="C29" s="40"/>
     </row>
     <row r="42" ht="14.25">
       <c r="B42" s="22"/>
@@ -3309,7 +3327,16 @@
       <c r="H43" s="40"/>
     </row>
     <row r="44" ht="14.25">
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
       <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="40"/>
+    </row>
+    <row r="45" ht="14.25">
+      <c r="E45" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Change attitude estimation algorithm
</commit_message>
<xml_diff>
--- a/Document/Protocol.xlsx
+++ b/Document/Protocol.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="238">
   <si>
     <t xml:space="preserve">Abbreviation List</t>
   </si>
@@ -609,15 +609,6 @@
     <t xml:space="preserve">Covariance matrix of measurement noise</t>
   </si>
   <si>
-    <t>0x38</t>
-  </si>
-  <si>
-    <t>DAT_HPF_ACC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High-pass filtered acceleration</t>
-  </si>
-  <si>
     <t>0x40</t>
   </si>
   <si>
@@ -691,6 +682,78 @@
   </si>
   <si>
     <t xml:space="preserve">RF received data channel 8</t>
+  </si>
+  <si>
+    <t>0x48</t>
+  </si>
+  <si>
+    <t>DAT_RF_CH9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF received data channel 9</t>
+  </si>
+  <si>
+    <t>0x49</t>
+  </si>
+  <si>
+    <t>DAT_RF_CH10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF received data channel 10</t>
+  </si>
+  <si>
+    <t>0x4A</t>
+  </si>
+  <si>
+    <t>DAT_RF_CH11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF received data channel 11</t>
+  </si>
+  <si>
+    <t>0x4B</t>
+  </si>
+  <si>
+    <t>DAT_RF_CH12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF received data channel 12</t>
+  </si>
+  <si>
+    <t>0x4C</t>
+  </si>
+  <si>
+    <t>DAT_RF_CH13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF received data channel 13</t>
+  </si>
+  <si>
+    <t>0x4D</t>
+  </si>
+  <si>
+    <t>DAT_RF_CH14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF received data channel 14</t>
+  </si>
+  <si>
+    <t>0x4E</t>
+  </si>
+  <si>
+    <t>DAT_RF_CH15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF received data channel 15</t>
+  </si>
+  <si>
+    <t>0x4F</t>
+  </si>
+  <si>
+    <t>DAT_RF_CH16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF received data channel 16</t>
   </si>
 </sst>
 </file>
@@ -3354,41 +3417,41 @@
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="58" t="s">
         <v>189</v>
       </c>
       <c r="C22" s="32">
-        <v>12</v>
-      </c>
-      <c r="D22" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="58" t="s">
         <v>190</v>
       </c>
-      <c r="E22" s="32" t="s">
+      <c r="E22" s="58" t="s">
         <v>191</v>
       </c>
-      <c r="F22" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="G22" s="32" t="s">
-        <v>141</v>
+      <c r="F22" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="G22" s="58" t="s">
+        <v>34</v>
       </c>
       <c r="H22" s="37"/>
     </row>
     <row r="23" ht="14.25">
       <c r="B23" s="58" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C23" s="32">
         <v>4</v>
       </c>
       <c r="D23" s="58" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E23" s="58" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F23" s="58" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G23" s="58" t="s">
         <v>34</v>
@@ -3409,7 +3472,7 @@
         <v>198</v>
       </c>
       <c r="F24" s="58" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G24" s="58" t="s">
         <v>34</v>
@@ -3430,7 +3493,7 @@
         <v>201</v>
       </c>
       <c r="F25" s="58" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G25" s="58" t="s">
         <v>34</v>
@@ -3451,7 +3514,7 @@
         <v>204</v>
       </c>
       <c r="F26" s="58" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G26" s="58" t="s">
         <v>34</v>
@@ -3472,7 +3535,7 @@
         <v>207</v>
       </c>
       <c r="F27" s="58" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G27" s="58" t="s">
         <v>34</v>
@@ -3483,7 +3546,7 @@
       <c r="B28" s="58" t="s">
         <v>208</v>
       </c>
-      <c r="C28" s="32">
+      <c r="C28" s="36">
         <v>4</v>
       </c>
       <c r="D28" s="58" t="s">
@@ -3493,7 +3556,7 @@
         <v>210</v>
       </c>
       <c r="F28" s="58" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G28" s="58" t="s">
         <v>34</v>
@@ -3504,7 +3567,7 @@
       <c r="B29" s="58" t="s">
         <v>211</v>
       </c>
-      <c r="C29" s="36">
+      <c r="C29" s="32">
         <v>4</v>
       </c>
       <c r="D29" s="58" t="s">
@@ -3514,7 +3577,7 @@
         <v>213</v>
       </c>
       <c r="F29" s="58" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G29" s="58" t="s">
         <v>34</v>
@@ -3525,7 +3588,7 @@
       <c r="B30" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="C30" s="32">
+      <c r="C30" s="36">
         <v>4</v>
       </c>
       <c r="D30" s="58" t="s">
@@ -3535,15 +3598,192 @@
         <v>216</v>
       </c>
       <c r="F30" s="58" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G30" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="H30" s="37"/>
+      <c r="H30" s="36"/>
     </row>
     <row r="31" ht="14.25">
-      <c r="B31" s="22"/>
+      <c r="B31" s="58" t="s">
+        <v>217</v>
+      </c>
+      <c r="C31" s="32">
+        <v>4</v>
+      </c>
+      <c r="D31" s="58" t="s">
+        <v>218</v>
+      </c>
+      <c r="E31" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="F31" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="G31" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="36"/>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="B32" s="58" t="s">
+        <v>220</v>
+      </c>
+      <c r="C32" s="36">
+        <v>4</v>
+      </c>
+      <c r="D32" s="58" t="s">
+        <v>221</v>
+      </c>
+      <c r="E32" s="58" t="s">
+        <v>222</v>
+      </c>
+      <c r="F32" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="G32" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="36"/>
+    </row>
+    <row r="33" ht="14.25">
+      <c r="B33" s="58" t="s">
+        <v>223</v>
+      </c>
+      <c r="C33" s="32">
+        <v>4</v>
+      </c>
+      <c r="D33" s="58" t="s">
+        <v>224</v>
+      </c>
+      <c r="E33" s="58" t="s">
+        <v>225</v>
+      </c>
+      <c r="F33" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="G33" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="36"/>
+    </row>
+    <row r="34" ht="14.25">
+      <c r="B34" s="58" t="s">
+        <v>226</v>
+      </c>
+      <c r="C34" s="36">
+        <v>4</v>
+      </c>
+      <c r="D34" s="58" t="s">
+        <v>227</v>
+      </c>
+      <c r="E34" s="58" t="s">
+        <v>228</v>
+      </c>
+      <c r="F34" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="G34" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" s="36"/>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="B35" s="58" t="s">
+        <v>229</v>
+      </c>
+      <c r="C35" s="32">
+        <v>4</v>
+      </c>
+      <c r="D35" s="58" t="s">
+        <v>230</v>
+      </c>
+      <c r="E35" s="58" t="s">
+        <v>231</v>
+      </c>
+      <c r="F35" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="G35" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="H35" s="36"/>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="B36" s="58" t="s">
+        <v>232</v>
+      </c>
+      <c r="C36" s="36">
+        <v>4</v>
+      </c>
+      <c r="D36" s="58" t="s">
+        <v>233</v>
+      </c>
+      <c r="E36" s="58" t="s">
+        <v>234</v>
+      </c>
+      <c r="F36" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="G36" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" s="36"/>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="B37" s="58" t="s">
+        <v>235</v>
+      </c>
+      <c r="C37" s="32">
+        <v>4</v>
+      </c>
+      <c r="D37" s="58" t="s">
+        <v>236</v>
+      </c>
+      <c r="E37" s="58" t="s">
+        <v>237</v>
+      </c>
+      <c r="F37" s="58" t="s">
+        <v>192</v>
+      </c>
+      <c r="G37" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="H37" s="36"/>
+    </row>
+    <row r="38" ht="14.25">
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+    </row>
+    <row r="39" ht="14.25">
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+    </row>
+    <row r="40" ht="14.25">
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="40"/>
+    </row>
+    <row r="41" ht="14.25">
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="40"/>
     </row>
     <row r="42" ht="14.25">
       <c r="B42" s="22"/>
@@ -3555,25 +3795,7 @@
       <c r="H42" s="40"/>
     </row>
     <row r="43" ht="14.25">
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
       <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="40"/>
-    </row>
-    <row r="44" ht="14.25">
-      <c r="B44" s="22"/>
-      <c r="C44" s="22"/>
-      <c r="D44" s="22"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="40"/>
-    </row>
-    <row r="45" ht="14.25">
-      <c r="E45" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Add motor control based on RF
</commit_message>
<xml_diff>
--- a/Document/Protocol.xlsx
+++ b/Document/Protocol.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="239">
   <si>
     <t xml:space="preserve">Abbreviation List</t>
   </si>
@@ -609,6 +609,9 @@
     <t xml:space="preserve">Covariance matrix of measurement noise</t>
   </si>
   <si>
+    <t>float[6][6]</t>
+  </si>
+  <si>
     <t>0x40</t>
   </si>
   <si>
@@ -762,29 +765,29 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <b/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11.000000"/>
+      <color theme="1"/>
       <name val="Calibri Light"/>
-      <color theme="1"/>
-      <sz val="11.000000"/>
       <scheme val="major"/>
     </font>
     <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color indexed="2"/>
       <name val="Calibri Light"/>
-      <b/>
-      <color indexed="2"/>
-      <sz val="11.000000"/>
       <scheme val="major"/>
     </font>
   </fonts>
@@ -1772,7 +1775,7 @@
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2066,7 +2069,7 @@
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2634,7 +2637,7 @@
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -2992,7 +2995,7 @@
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -3406,8 +3409,8 @@
       <c r="E21" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="F21" s="32" t="s">
-        <v>181</v>
+      <c r="F21" s="58" t="s">
+        <v>189</v>
       </c>
       <c r="G21" s="32" t="s">
         <v>34</v>
@@ -3417,337 +3420,337 @@
       </c>
     </row>
     <row r="22" ht="14.25">
-      <c r="B22" s="58" t="s">
-        <v>189</v>
+      <c r="B22" s="32" t="s">
+        <v>190</v>
       </c>
       <c r="C22" s="32">
         <v>4</v>
       </c>
-      <c r="D22" s="58" t="s">
-        <v>190</v>
-      </c>
-      <c r="E22" s="58" t="s">
+      <c r="D22" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="F22" s="58" t="s">
+      <c r="E22" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="G22" s="58" t="s">
+      <c r="F22" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G22" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H22" s="37"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="B23" s="58" t="s">
-        <v>193</v>
+      <c r="B23" s="32" t="s">
+        <v>194</v>
       </c>
       <c r="C23" s="32">
         <v>4</v>
       </c>
-      <c r="D23" s="58" t="s">
-        <v>194</v>
-      </c>
-      <c r="E23" s="58" t="s">
+      <c r="D23" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="F23" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G23" s="58" t="s">
+      <c r="E23" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G23" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H23" s="37"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="B24" s="58" t="s">
-        <v>196</v>
+      <c r="B24" s="32" t="s">
+        <v>197</v>
       </c>
       <c r="C24" s="32">
         <v>4</v>
       </c>
-      <c r="D24" s="58" t="s">
-        <v>197</v>
-      </c>
-      <c r="E24" s="58" t="s">
+      <c r="D24" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="F24" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G24" s="58" t="s">
+      <c r="E24" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G24" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H24" s="37"/>
     </row>
     <row r="25" ht="14.25">
-      <c r="B25" s="58" t="s">
-        <v>199</v>
+      <c r="B25" s="32" t="s">
+        <v>200</v>
       </c>
       <c r="C25" s="32">
         <v>4</v>
       </c>
-      <c r="D25" s="58" t="s">
-        <v>200</v>
-      </c>
-      <c r="E25" s="58" t="s">
+      <c r="D25" s="32" t="s">
         <v>201</v>
       </c>
-      <c r="F25" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G25" s="58" t="s">
+      <c r="E25" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G25" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H25" s="37"/>
     </row>
     <row r="26" ht="14.25">
-      <c r="B26" s="58" t="s">
-        <v>202</v>
+      <c r="B26" s="32" t="s">
+        <v>203</v>
       </c>
       <c r="C26" s="32">
         <v>4</v>
       </c>
-      <c r="D26" s="58" t="s">
-        <v>203</v>
-      </c>
-      <c r="E26" s="58" t="s">
+      <c r="D26" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="F26" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G26" s="58" t="s">
+      <c r="E26" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G26" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H26" s="37"/>
     </row>
     <row r="27" ht="14.25">
-      <c r="B27" s="58" t="s">
-        <v>205</v>
+      <c r="B27" s="32" t="s">
+        <v>206</v>
       </c>
       <c r="C27" s="32">
         <v>4</v>
       </c>
-      <c r="D27" s="58" t="s">
-        <v>206</v>
-      </c>
-      <c r="E27" s="58" t="s">
+      <c r="D27" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="F27" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G27" s="58" t="s">
+      <c r="E27" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G27" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H27" s="37"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="B28" s="58" t="s">
-        <v>208</v>
+      <c r="B28" s="32" t="s">
+        <v>209</v>
       </c>
       <c r="C28" s="36">
         <v>4</v>
       </c>
-      <c r="D28" s="58" t="s">
-        <v>209</v>
-      </c>
-      <c r="E28" s="58" t="s">
+      <c r="D28" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="F28" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G28" s="58" t="s">
+      <c r="E28" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G28" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H28" s="37"/>
     </row>
     <row r="29" ht="14.25">
-      <c r="B29" s="58" t="s">
-        <v>211</v>
+      <c r="B29" s="32" t="s">
+        <v>212</v>
       </c>
       <c r="C29" s="32">
         <v>4</v>
       </c>
-      <c r="D29" s="58" t="s">
-        <v>212</v>
-      </c>
-      <c r="E29" s="58" t="s">
+      <c r="D29" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="F29" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G29" s="58" t="s">
+      <c r="E29" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G29" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H29" s="37"/>
     </row>
     <row r="30" ht="14.25">
-      <c r="B30" s="58" t="s">
-        <v>214</v>
+      <c r="B30" s="32" t="s">
+        <v>215</v>
       </c>
       <c r="C30" s="36">
         <v>4</v>
       </c>
-      <c r="D30" s="58" t="s">
-        <v>215</v>
-      </c>
-      <c r="E30" s="58" t="s">
+      <c r="D30" s="32" t="s">
         <v>216</v>
       </c>
-      <c r="F30" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G30" s="58" t="s">
+      <c r="E30" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G30" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H30" s="36"/>
     </row>
     <row r="31" ht="14.25">
-      <c r="B31" s="58" t="s">
-        <v>217</v>
+      <c r="B31" s="32" t="s">
+        <v>218</v>
       </c>
       <c r="C31" s="32">
         <v>4</v>
       </c>
-      <c r="D31" s="58" t="s">
-        <v>218</v>
-      </c>
-      <c r="E31" s="58" t="s">
+      <c r="D31" s="32" t="s">
         <v>219</v>
       </c>
-      <c r="F31" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G31" s="58" t="s">
+      <c r="E31" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G31" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H31" s="36"/>
     </row>
     <row r="32" ht="14.25">
-      <c r="B32" s="58" t="s">
-        <v>220</v>
+      <c r="B32" s="32" t="s">
+        <v>221</v>
       </c>
       <c r="C32" s="36">
         <v>4</v>
       </c>
-      <c r="D32" s="58" t="s">
-        <v>221</v>
-      </c>
-      <c r="E32" s="58" t="s">
+      <c r="D32" s="32" t="s">
         <v>222</v>
       </c>
-      <c r="F32" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G32" s="58" t="s">
+      <c r="E32" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="F32" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G32" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H32" s="36"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="B33" s="58" t="s">
-        <v>223</v>
+      <c r="B33" s="32" t="s">
+        <v>224</v>
       </c>
       <c r="C33" s="32">
         <v>4</v>
       </c>
-      <c r="D33" s="58" t="s">
-        <v>224</v>
-      </c>
-      <c r="E33" s="58" t="s">
+      <c r="D33" s="32" t="s">
         <v>225</v>
       </c>
-      <c r="F33" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G33" s="58" t="s">
+      <c r="E33" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G33" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H33" s="36"/>
     </row>
     <row r="34" ht="14.25">
-      <c r="B34" s="58" t="s">
-        <v>226</v>
+      <c r="B34" s="32" t="s">
+        <v>227</v>
       </c>
       <c r="C34" s="36">
         <v>4</v>
       </c>
-      <c r="D34" s="58" t="s">
-        <v>227</v>
-      </c>
-      <c r="E34" s="58" t="s">
+      <c r="D34" s="32" t="s">
         <v>228</v>
       </c>
-      <c r="F34" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G34" s="58" t="s">
+      <c r="E34" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="F34" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G34" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H34" s="36"/>
     </row>
     <row r="35" ht="14.25">
-      <c r="B35" s="58" t="s">
-        <v>229</v>
+      <c r="B35" s="32" t="s">
+        <v>230</v>
       </c>
       <c r="C35" s="32">
         <v>4</v>
       </c>
-      <c r="D35" s="58" t="s">
-        <v>230</v>
-      </c>
-      <c r="E35" s="58" t="s">
+      <c r="D35" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="F35" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G35" s="58" t="s">
+      <c r="E35" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="F35" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G35" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H35" s="36"/>
     </row>
     <row r="36" ht="14.25">
-      <c r="B36" s="58" t="s">
-        <v>232</v>
+      <c r="B36" s="32" t="s">
+        <v>233</v>
       </c>
       <c r="C36" s="36">
         <v>4</v>
       </c>
-      <c r="D36" s="58" t="s">
-        <v>233</v>
-      </c>
-      <c r="E36" s="58" t="s">
+      <c r="D36" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="F36" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G36" s="58" t="s">
+      <c r="E36" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="F36" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G36" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H36" s="36"/>
     </row>
     <row r="37" ht="14.25">
-      <c r="B37" s="58" t="s">
-        <v>235</v>
+      <c r="B37" s="32" t="s">
+        <v>236</v>
       </c>
       <c r="C37" s="32">
         <v>4</v>
       </c>
-      <c r="D37" s="58" t="s">
-        <v>236</v>
-      </c>
-      <c r="E37" s="58" t="s">
+      <c r="D37" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="F37" s="58" t="s">
-        <v>192</v>
-      </c>
-      <c r="G37" s="58" t="s">
+      <c r="E37" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="F37" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="G37" s="32" t="s">
         <v>34</v>
       </c>
       <c r="H37" s="36"/>
@@ -3804,7 +3807,7 @@
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>